<commit_message>
Skończono rozdział 6 - opisano integrację z bazą i załadowanie danych
</commit_message>
<xml_diff>
--- a/BazaDanych/movies.xlsx
+++ b/BazaDanych/movies.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michal\Desktop\Inżynierka\BazaDanych\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Moje dane\Studia\PracaInzynierska\BazaDanych\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43469F4D-D380-4745-BC93-37B775649133}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4DE68C0-C4D2-499A-AA37-6ED3E770122D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -996,13 +996,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperłącze" xfId="1" builtinId="8"/>
@@ -1287,20 +1286,20 @@
   <dimension ref="A1:J46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q16" sqref="Q16"/>
+      <selection activeCell="R17" sqref="R17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="30.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="29.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="21" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="6.140625" style="1" customWidth="1"/>
     <col min="7" max="7" width="8.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="26" style="1" customWidth="1"/>
-    <col min="9" max="9" width="8.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14" style="1" customWidth="1"/>
     <col min="10" max="10" width="15.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1355,7 +1354,7 @@
       <c r="F2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" t="s">
         <v>258</v>
       </c>
       <c r="H2" s="1" t="s">

</xml_diff>